<commit_message>
[ADD] Added service that changes the schedule every monday at 00:01
</commit_message>
<xml_diff>
--- a/public/semana_siguiente.xlsx
+++ b/public/semana_siguiente.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ruymy\Documents\TFG\StorageCSR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ruymy\Documents\TFG\StorageCSR\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4372668-8197-43DD-A83D-55F16BE2970E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CB7059-70E6-459C-9326-6EDE3A417A1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A0371084-3A69-4FBF-931F-C13DD5562A6A}"/>
+    <workbookView xWindow="-5220" yWindow="-15870" windowWidth="29040" windowHeight="15990" xr2:uid="{A0371084-3A69-4FBF-931F-C13DD5562A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Timestamp_final</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>02:15</t>
+  </si>
+  <si>
+    <t>0_mkma36fu</t>
   </si>
 </sst>
 </file>
@@ -446,7 +455,7 @@
   <dimension ref="A1:E602"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E8"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,11 +486,17 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>

</xml_diff>